<commit_message>
validetion for all and fix bugs
</commit_message>
<xml_diff>
--- a/HabitatBirdsApplication/HabitatBirdsApplication/bin/Debug/net6.0-windows/Data/Birds.xlsx
+++ b/HabitatBirdsApplication/HabitatBirdsApplication/bin/Debug/net6.0-windows/Data/Birds.xlsx
@@ -3,8 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Osnat\Desktop\HabitatBirds\HabitatBirdsApplication\HabitatBirdsApplication\bin\Debug\net6.0-windows\Data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2042D1B6-C8C3-446A-9026-22C7A70E0D33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" activeTab="2"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="16200" windowHeight="9270" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -13,11 +19,11 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" chartTrackingRefBase="1"/>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures">
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
@@ -32,126 +38,96 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="69">
-  <si>
-    <t xml:space="preserve">First Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Last Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Password</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nmfd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dfjk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">123456789</t>
-  </si>
-  <si>
-    <t xml:space="preserve">matanih</t>
-  </si>
-  <si>
-    <t xml:space="preserve">!1m123456</t>
-  </si>
-  <si>
-    <t xml:space="preserve">buga</t>
-  </si>
-  <si>
-    <t xml:space="preserve">joni</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jonibuga</t>
-  </si>
-  <si>
-    <t xml:space="preserve">!1b12345</t>
-  </si>
-  <si>
-    <t xml:space="preserve">matan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nitzan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">matani</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mbbhg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nbmjh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TaliaEl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1!t12345</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Serial</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Material</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Length</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Witdh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Height</t>
-  </si>
-  <si>
-    <t xml:space="preserve">134f</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Iron</t>
-  </si>
-  <si>
-    <t xml:space="preserve">134fjj</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wood</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23dff</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Plastic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23djon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">132ks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">123ff</t>
-  </si>
-  <si>
-    <t xml:space="preserve">134ju</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5ss</t>
-  </si>
-  <si>
-    <t xml:space="preserve">298y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">45ff</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Serial number</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="76">
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>User Name</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>nmfd</t>
+  </si>
+  <si>
+    <t>dfjk</t>
+  </si>
+  <si>
+    <t>123456789</t>
+  </si>
+  <si>
+    <t>matanih</t>
+  </si>
+  <si>
+    <t>!1m123456</t>
+  </si>
+  <si>
+    <t>buga</t>
+  </si>
+  <si>
+    <t>joni</t>
+  </si>
+  <si>
+    <t>jonibuga</t>
+  </si>
+  <si>
+    <t>!1b12345</t>
+  </si>
+  <si>
+    <t>matan</t>
+  </si>
+  <si>
+    <t>nitzan</t>
+  </si>
+  <si>
+    <t>matani</t>
+  </si>
+  <si>
+    <t>mbbhg</t>
+  </si>
+  <si>
+    <t>nbmjh</t>
+  </si>
+  <si>
+    <t>TaliaEl</t>
+  </si>
+  <si>
+    <t>1!t12345</t>
+  </si>
+  <si>
+    <t>Serial</t>
+  </si>
+  <si>
+    <t>Material</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>Witdh</t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>Iron</t>
+  </si>
+  <si>
+    <t>Wood</t>
+  </si>
+  <si>
+    <t>Plastic</t>
+  </si>
+  <si>
+    <t>Serial number</t>
   </si>
   <si>
     <t xml:space="preserve"> The species of the bird</t>
@@ -163,90 +139,140 @@
     <t xml:space="preserve"> Hatch date</t>
   </si>
   <si>
-    <t xml:space="preserve">Gander</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cage numbe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Father's serial number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mother's serial number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Username</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">American Gouldian</t>
-  </si>
-  <si>
-    <t xml:space="preserve">North America</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Male</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1435A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Has chicks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Female</t>
-  </si>
-  <si>
-    <t xml:space="preserve">60</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FALSE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TRUE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">90</t>
-  </si>
-  <si>
-    <t xml:space="preserve">28</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1342K</t>
-  </si>
-  <si>
-    <t xml:space="preserve">777</t>
-  </si>
-  <si>
-    <t xml:space="preserve">200</t>
-  </si>
-  <si>
-    <t xml:space="preserve"/>
-  </si>
-  <si>
-    <t xml:space="preserve">12334</t>
+    <t>Gander</t>
+  </si>
+  <si>
+    <t>Cage numbe</t>
+  </si>
+  <si>
+    <t>Father's serial number</t>
+  </si>
+  <si>
+    <t>Mother's serial number</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>American Gouldian</t>
+  </si>
+  <si>
+    <t>North America</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Has chicks</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>FALSE</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>TRUE</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>777</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>osnat</t>
+  </si>
+  <si>
+    <t>shabtay</t>
+  </si>
+  <si>
+    <t>osnat1</t>
+  </si>
+  <si>
+    <t>1!o12345</t>
+  </si>
+  <si>
+    <t>shabbtay</t>
+  </si>
+  <si>
+    <t>osnat11</t>
+  </si>
+  <si>
+    <t>Moshe</t>
+  </si>
+  <si>
+    <t>Davidyan</t>
+  </si>
+  <si>
+    <t>MosheD</t>
+  </si>
+  <si>
+    <t>1!m12345</t>
+  </si>
+  <si>
+    <t>A14</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>A5</t>
+  </si>
+  <si>
+    <t>A6</t>
+  </si>
+  <si>
+    <t>A7</t>
+  </si>
+  <si>
+    <t>A8</t>
+  </si>
+  <si>
+    <t>A9</t>
+  </si>
+  <si>
+    <t>A10</t>
+  </si>
+  <si>
+    <t>A11</t>
+  </si>
+  <si>
+    <t>A12</t>
+  </si>
+  <si>
+    <t>A13</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -266,6 +292,12 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -295,7 +327,7 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -319,30 +351,18 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -637,8 +657,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1:E5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
@@ -737,20 +757,69 @@
         <v>20</v>
       </c>
     </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" t="s">
+        <v>61</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <headerFooter/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1:E12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -774,10 +843,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" t="s">
         <v>26</v>
-      </c>
-      <c r="B2" t="s">
-        <v>27</v>
       </c>
       <c r="C2">
         <v>434</v>
@@ -791,10 +860,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>63</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C3">
         <v>12</v>
@@ -808,10 +877,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>64</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C4">
         <v>14</v>
@@ -825,10 +894,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>65</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C5">
         <v>14</v>
@@ -842,10 +911,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>67</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C6">
         <v>21</v>
@@ -859,10 +928,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>68</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7">
         <v>12</v>
@@ -876,10 +945,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>69</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C8">
         <v>243</v>
@@ -893,10 +962,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>70</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C9">
         <v>12</v>
@@ -910,10 +979,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>71</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C10">
         <v>23</v>
@@ -927,10 +996,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>72</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C11">
         <v>43</v>
@@ -944,13 +1013,13 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>55</v>
+        <v>73</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C12">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="D12">
         <v>500</v>
@@ -959,12 +1028,12 @@
         <v>600</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C13">
         <v>400</v>
@@ -976,20 +1045,51 @@
         <v>70</v>
       </c>
     </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>75</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14">
+        <v>211</v>
+      </c>
+      <c r="D14">
+        <v>122</v>
+      </c>
+      <c r="E14">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15">
+        <v>12</v>
+      </c>
+      <c r="D15">
+        <v>122</v>
+      </c>
+      <c r="E15">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="default"/>
-  <headerFooter/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1:J9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1006,330 +1106,415 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="7">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C2" t="s">
         <v>40</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" t="s">
-        <v>50</v>
       </c>
       <c r="D2" s="5">
         <v>45058</v>
       </c>
       <c r="E2" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="F2" t="s">
-        <v>32</v>
+        <v>71</v>
       </c>
       <c r="G2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J2" t="s">
         <v>48</v>
       </c>
-      <c r="H2" t="s">
-        <v>48</v>
-      </c>
-      <c r="J2" t="b">
-        <v>0</v>
-      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>54</v>
+      <c r="A3" s="7">
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D3" s="5">
         <v>45058</v>
       </c>
       <c r="E3" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="F3" t="s">
-        <v>37</v>
+        <v>71</v>
       </c>
       <c r="G3" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="H3" t="s">
-        <v>54</v>
-      </c>
-      <c r="J3" t="b">
-        <v>0</v>
+        <v>42</v>
+      </c>
+      <c r="J3" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="C4" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D4" s="5">
         <v>45058</v>
       </c>
       <c r="E4" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="F4" t="s">
-        <v>26</v>
+        <v>73</v>
       </c>
       <c r="G4" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="H4" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="J4" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D5" s="5">
-        <v>45058</v>
+        <v>45076</v>
       </c>
       <c r="E5" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="F5" t="s">
-        <v>26</v>
+        <v>73</v>
       </c>
       <c r="G5" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="H5" t="s">
-        <v>53</v>
-      </c>
-      <c r="J5" t="b">
-        <v>0</v>
+        <v>47</v>
+      </c>
+      <c r="J5" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
-        <v>28</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="5">
+        <v>45075</v>
+      </c>
+      <c r="E6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" t="s">
+        <v>73</v>
+      </c>
+      <c r="G6" t="s">
         <v>49</v>
       </c>
-      <c r="C6" t="s">
+      <c r="H6" t="s">
+        <v>47</v>
+      </c>
+      <c r="J6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="5">
+        <v>45054</v>
+      </c>
+      <c r="E7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" t="s">
+        <v>73</v>
+      </c>
+      <c r="G7" t="s">
         <v>50</v>
       </c>
-      <c r="D6" s="5">
+      <c r="H7" t="s">
+        <v>50</v>
+      </c>
+      <c r="J7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="5">
+        <v>45051</v>
+      </c>
+      <c r="E8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" t="s">
+        <v>74</v>
+      </c>
+      <c r="G8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H8" t="s">
+        <v>50</v>
+      </c>
+      <c r="J8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="5">
+        <v>45064</v>
+      </c>
+      <c r="E9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" t="s">
+        <v>73</v>
+      </c>
+      <c r="G9" t="s">
+        <v>50</v>
+      </c>
+      <c r="H9" t="s">
+        <v>50</v>
+      </c>
+      <c r="J9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="5">
         <v>45058</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" t="s">
+        <v>70</v>
+      </c>
+      <c r="G10" t="s">
+        <v>38</v>
+      </c>
+      <c r="H10" t="s">
+        <v>38</v>
+      </c>
+      <c r="J10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="5">
+        <v>45072</v>
+      </c>
+      <c r="E11" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" t="s">
+        <v>70</v>
+      </c>
+      <c r="G11" t="s">
+        <v>45</v>
+      </c>
+      <c r="H11" t="s">
+        <v>47</v>
+      </c>
+      <c r="J11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="5">
+        <v>45077</v>
+      </c>
+      <c r="E12" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" t="s">
+        <v>70</v>
+      </c>
+      <c r="G12" t="s">
+        <v>50</v>
+      </c>
+      <c r="H12" t="s">
+        <v>50</v>
+      </c>
+      <c r="J12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="5">
+        <v>45058</v>
+      </c>
+      <c r="E13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" t="s">
+        <v>70</v>
+      </c>
+      <c r="G13" t="s">
+        <v>50</v>
+      </c>
+      <c r="H13" t="s">
+        <v>50</v>
+      </c>
+      <c r="J13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="5">
+        <v>45050</v>
+      </c>
+      <c r="E14" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" t="s">
+        <v>71</v>
+      </c>
+      <c r="G14" t="s">
         <v>51</v>
       </c>
-      <c r="F6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" t="s">
-        <v>53</v>
-      </c>
-      <c r="H6" t="s">
-        <v>53</v>
-      </c>
-      <c r="J6" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="B7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7" t="s">
-        <v>50</v>
-      </c>
-      <c r="D7" s="5">
-        <v>45076</v>
-      </c>
-      <c r="E7" t="s">
-        <v>51</v>
-      </c>
-      <c r="F7" t="s">
-        <v>26</v>
-      </c>
-      <c r="G7" t="s">
-        <v>53</v>
-      </c>
-      <c r="H7" t="s">
-        <v>60</v>
-      </c>
-      <c r="J7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="B8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C8" t="s">
-        <v>50</v>
-      </c>
-      <c r="D8" s="5">
-        <v>45075</v>
-      </c>
-      <c r="E8" t="s">
-        <v>57</v>
-      </c>
-      <c r="F8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G8" t="s">
-        <v>63</v>
-      </c>
-      <c r="H8" t="s">
-        <v>60</v>
-      </c>
-      <c r="J8" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="B9" t="s">
-        <v>49</v>
-      </c>
-      <c r="C9" t="s">
-        <v>50</v>
-      </c>
-      <c r="D9" s="5">
-        <v>45055</v>
-      </c>
-      <c r="E9" t="s">
-        <v>51</v>
-      </c>
-      <c r="F9" t="s">
-        <v>26</v>
-      </c>
-      <c r="G9" t="s">
-        <v>65</v>
-      </c>
-      <c r="H9" t="s">
-        <v>65</v>
-      </c>
-      <c r="J9" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="B10" t="s">
-        <v>49</v>
-      </c>
-      <c r="C10" t="s">
-        <v>50</v>
-      </c>
-      <c r="D10" s="5">
-        <v>45054</v>
-      </c>
-      <c r="E10" t="s">
-        <v>51</v>
-      </c>
-      <c r="F10" t="s">
-        <v>26</v>
-      </c>
-      <c r="G10" t="s">
-        <v>65</v>
-      </c>
-      <c r="H10" t="s">
-        <v>65</v>
-      </c>
-      <c r="J10" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="B11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C11" t="s">
-        <v>50</v>
-      </c>
-      <c r="D11" s="5">
-        <v>45051</v>
-      </c>
-      <c r="E11" t="s">
-        <v>51</v>
-      </c>
-      <c r="F11" t="s">
-        <v>26</v>
-      </c>
-      <c r="G11" t="s">
-        <v>65</v>
-      </c>
-      <c r="H11" t="s">
-        <v>65</v>
-      </c>
-      <c r="J11" t="s">
-        <v>59</v>
+      <c r="H14" t="s">
+        <v>47</v>
+      </c>
+      <c r="J14" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="default"/>
-  <headerFooter/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>